<commit_message>
made many changes condensed things a lot
NB: note to all please change the filepaths in each to where it is saved on your computer
</commit_message>
<xml_diff>
--- a/data/solvay_attributes.xlsx
+++ b/data/solvay_attributes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer internship/pycharm_factory/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer internship/FUSE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A384C8-E4AE-7440-A5F9-406862A7F57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40957BC5-8235-FD40-BB5D-A3C95F78B202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" firstSheet="5" activeTab="9" xr2:uid="{9721A122-EEC0-DB4B-B0DC-E98509EB2D90}"/>
+    <workbookView xWindow="44340" yWindow="-1860" windowWidth="14280" windowHeight="17500" firstSheet="5" activeTab="8" xr2:uid="{9721A122-EEC0-DB4B-B0DC-E98509EB2D90}"/>
   </bookViews>
   <sheets>
     <sheet name="brine" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="25">
   <si>
     <t>key</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>reactor volume</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78269108-B176-8D4B-AA03-F1F572BCD5A3}">
   <dimension ref="A2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -1034,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BF4165-714F-6C4D-BD52-5A2477EDFAD6}">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,7 +1064,7 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -1072,10 +1075,21 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>848.2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
still moving things about
</commit_message>
<xml_diff>
--- a/data/solvay_attributes.xlsx
+++ b/data/solvay_attributes.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer internship/FUSE/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer work experience/Imperial College/FUSE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4587D51-B67F-5141-A7AE-348A0D84BC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A992C5E-6095-2B49-8380-260D018F8E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34660" yWindow="-2060" windowWidth="27940" windowHeight="17500" xr2:uid="{9721A122-EEC0-DB4B-B0DC-E98509EB2D90}"/>
+    <workbookView xWindow="180" yWindow="500" windowWidth="17020" windowHeight="17500" activeTab="1" xr2:uid="{9721A122-EEC0-DB4B-B0DC-E98509EB2D90}"/>
   </bookViews>
   <sheets>
     <sheet name="brine" sheetId="1" r:id="rId1"/>
-    <sheet name="ammonia" sheetId="4" r:id="rId2"/>
-    <sheet name="limestone" sheetId="2" r:id="rId3"/>
-    <sheet name="coke" sheetId="3" r:id="rId4"/>
-    <sheet name="lime kiln" sheetId="5" r:id="rId5"/>
-    <sheet name="ammonia saturator" sheetId="6" r:id="rId6"/>
-    <sheet name="slacker" sheetId="7" r:id="rId7"/>
-    <sheet name="filter" sheetId="8" r:id="rId8"/>
-    <sheet name="calciner" sheetId="9" r:id="rId9"/>
-    <sheet name="ammonia recovery tower" sheetId="10" r:id="rId10"/>
-    <sheet name="solvay tower" sheetId="11" r:id="rId11"/>
+    <sheet name="Solvay Plant" sheetId="12" r:id="rId2"/>
+    <sheet name="ammonia" sheetId="4" r:id="rId3"/>
+    <sheet name="limestone" sheetId="2" r:id="rId4"/>
+    <sheet name="coke" sheetId="3" r:id="rId5"/>
+    <sheet name="lime kiln" sheetId="5" r:id="rId6"/>
+    <sheet name="ammonia saturator" sheetId="6" r:id="rId7"/>
+    <sheet name="slacker" sheetId="7" r:id="rId8"/>
+    <sheet name="filter" sheetId="8" r:id="rId9"/>
+    <sheet name="calciner" sheetId="9" r:id="rId10"/>
+    <sheet name="ammonia recovery tower" sheetId="10" r:id="rId11"/>
+    <sheet name="solvay tower" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="31">
   <si>
     <t>key</t>
   </si>
@@ -122,6 +123,21 @@
   </si>
   <si>
     <t>Source: https://www.scientificamerican.com/article/vanishing-baking-soda/</t>
+  </si>
+  <si>
+    <t>ammonia absorber</t>
+  </si>
+  <si>
+    <t>filter 1</t>
+  </si>
+  <si>
+    <t>solvay tower</t>
+  </si>
+  <si>
+    <t>lime kiln</t>
+  </si>
+  <si>
+    <t>slaker</t>
   </si>
 </sst>
 </file>
@@ -483,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BCA8696-8F25-C64F-AF6F-9E5CCBE8238C}">
   <dimension ref="A2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -550,6 +566,74 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BF4165-714F-6C4D-BD52-5A2477EDFAD6}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>0.25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>848.2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78269108-B176-8D4B-AA03-F1F572BCD5A3}">
   <dimension ref="A2:C18"/>
   <sheetViews>
@@ -630,7 +714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9864500C-A660-5F46-A703-A4B829594AFD}">
   <dimension ref="A2:C4"/>
   <sheetViews>
@@ -679,6 +763,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79F26FB-C160-F94E-B74E-65B051E1A38C}">
+  <dimension ref="A2:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B12228AE-BAD5-2D40-8399-B245EEBDF423}">
   <dimension ref="A2:C4"/>
   <sheetViews>
@@ -723,7 +847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B01BFF7-2D47-F748-8804-B88BC3D38360}">
   <dimension ref="A2:C4"/>
   <sheetViews>
@@ -768,7 +892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7691FE06-DD84-B945-B25A-F5CF00C8B90B}">
   <dimension ref="A2:C4"/>
   <sheetViews>
@@ -813,7 +937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD76B872-A295-3340-9F22-E722ECC2A21C}">
   <dimension ref="A2:C14"/>
   <sheetViews>
@@ -894,7 +1018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88148BF-4C23-4744-89C7-4D67A10BA1B1}">
   <dimension ref="A2:C4"/>
   <sheetViews>
@@ -942,7 +1066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97014EEF-F1C8-944F-A2A5-8E3E126ECBAD}">
   <dimension ref="A2:C4"/>
   <sheetViews>
@@ -990,7 +1114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF728BE7-5188-5049-8706-29EAFBB391F9}">
   <dimension ref="A2:C4"/>
   <sheetViews>
@@ -1036,72 +1160,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BF4165-714F-6C4D-BD52-5A2477EDFAD6}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4">
-        <v>0.25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>848.2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>